<commit_message>
insert excel to sqlserver
</commit_message>
<xml_diff>
--- a/wwwroot/files/Book1.xlsx
+++ b/wwwroot/files/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiti\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{256AC03A-1FF7-447C-AED1-E9F725A49760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C16E33-DE10-44B4-99D7-1E057B8B5AA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC966311-917F-4A34-871F-1D1BAD101358}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>qweqew</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>sssss</t>
+  </si>
+  <si>
+    <t>kaka</t>
+  </si>
+  <si>
+    <t>testja</t>
   </si>
 </sst>
 </file>
@@ -394,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8721F21A-D4C9-4F46-916B-EB527D06EE56}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,6 +441,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>